<commit_message>
make ExcelIO-Excel test pass :heavy_check_mark:
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_Excel.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_Excel.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\IO\FsSpreadsheet\tests\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EE117D-4835-4F86-808D-B1B3BFF52FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1E11E-B158-4269-8B17-EBBA9EEB720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </bookViews>
   <sheets>
     <sheet name="WithTable" sheetId="1" r:id="rId1"/>
-    <sheet name="Tableless" sheetId="2" r:id="rId2"/>
+    <sheet name="Tableless" sheetId="4" r:id="rId2"/>
     <sheet name="WithTable_Duplicate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -97,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -105,57 +105,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -203,7 +162,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -502,10 +461,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
@@ -536,7 +495,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>45213</v>
       </c>
       <c r="D2" t="s">
@@ -553,7 +512,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>45214</v>
       </c>
       <c r="E3" t="s">
@@ -567,7 +526,7 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>45215</v>
       </c>
     </row>
@@ -578,7 +537,7 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>45216</v>
       </c>
     </row>
@@ -591,14 +550,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C74DDE2-CDF5-40D3-9F40-97EED0BE5279}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C16715-9795-4E17-A00E-CEB100B9AE9C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -624,7 +586,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>45213</v>
       </c>
       <c r="D2" t="s">
@@ -641,7 +603,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>45214</v>
       </c>
       <c r="E3" t="s">
@@ -655,25 +617,23 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>45215</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>45216</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -685,7 +645,7 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -711,7 +671,7 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>45213</v>
       </c>
       <c r="E5" t="s">
@@ -728,7 +688,7 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>45214</v>
       </c>
       <c r="F6" t="s">
@@ -742,7 +702,7 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>45215</v>
       </c>
     </row>
@@ -753,7 +713,7 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>45216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start implementing logic for auto update, but push to backlog for now
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_Excel.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9724B-E1DD-4CE8-B902-5C9BA3C810AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5AFA2D-2952-483B-A3DB-C8DA3584682D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <workbookView xWindow="4395" yWindow="0" windowWidth="24510" windowHeight="15045" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </bookViews>
   <sheets>
     <sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>